<commit_message>
Cost of a 3-kilometer taxi ride in 88 major cities
Note for importing: data start at row number 5 (no header row)
source: https://www.priceoftravel.com/555/world-taxi-prices-what-a-3-kilometer-ride-costs-in-72-big-cities/
*All prices converted into US dollars on June 8, 2017
</commit_message>
<xml_diff>
--- a/taxi_rate_around_the_world.xlsx
+++ b/taxi_rate_around_the_world.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/prasert/Dropbox/Excel_Instructor/Exam/2017/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/prasert/Dropbox/Excel_Instructor/Exam_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,270 +29,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
   <si>
-    <t>$0.82 – $1.24 Delhi, India</t>
-  </si>
-  <si>
-    <t>$0.87 – $2.90 La Paz, Bolivia</t>
-  </si>
-  <si>
-    <t>$0.88 – $1.37 Mexico City, Mexico</t>
-  </si>
-  <si>
-    <t>$0.93 – $1.40 Mumbai, India</t>
-  </si>
-  <si>
-    <t>$1.03 – $2.05 Marrakech, Morocco</t>
-  </si>
-  <si>
-    <t>$1.09 – $1.63 Antigua, Guatemala</t>
-  </si>
-  <si>
-    <t>$1.21 – $1.62 Manila, Philippines</t>
-  </si>
-  <si>
-    <t>$1.41 – $2.34 Kuala Lumpur, Malaysia</t>
-  </si>
-  <si>
-    <t>$1.43 – $2.87 Zanzibar Town, Tanzania</t>
-  </si>
-  <si>
-    <t>$1.51 – $2.26 Kuta, Bali, Indonesia</t>
-  </si>
-  <si>
-    <t>$1.54 – $2.05 Fez, Morocco</t>
-  </si>
-  <si>
-    <t>$1.59 – $2.65 Ho Chi Minh City, Vietnam</t>
-  </si>
-  <si>
-    <t>$1.76 – $2.94 Bangkok, Thailand</t>
-  </si>
-  <si>
-    <t>$1.79 – $2.68 Yangon, Myanmar</t>
-  </si>
-  <si>
-    <t>$1.79 – $2.24 Arusha, Tanzania</t>
-  </si>
-  <si>
-    <t>$1.86 – $2.32 Cape Town, South Africa</t>
-  </si>
-  <si>
-    <t>$1.91 – $2.94 Beijing, China</t>
-  </si>
-  <si>
-    <t>$1.94 – $2.77 Cairo, Egypt</t>
-  </si>
-  <si>
-    <t>$1.98 – $3.09 Hanoi, Vietnam</t>
-  </si>
-  <si>
-    <t>$2.00 – $4.00 Quito, Ecuador</t>
-  </si>
-  <si>
-    <t>$2.25 – $3.27 Dubai, UAE</t>
-  </si>
-  <si>
-    <t>$2.27 – $4.25 Istanbul, Turkey</t>
-  </si>
-  <si>
-    <t>$2.28 – $2.43 Kathmandu, Nepal</t>
-  </si>
-  <si>
-    <t>$2.30 – $3.16 Sofia, Bulgaria</t>
-  </si>
-  <si>
-    <t>$2.50 – $3.38 Shanghai, China</t>
-  </si>
-  <si>
-    <t>$2.50 – $3.13 Buenos Aires, Argentina</t>
-  </si>
-  <si>
-    <t>$2.74 – $4.88 Rio de Janeiro, Brazil</t>
-  </si>
-  <si>
-    <t>$2.76 – $5.35 Seoul, South Korea</t>
-  </si>
-  <si>
-    <t>$2.81 – $3.51 Montevideo, Uruguay</t>
-  </si>
-  <si>
-    <t>$2.82 – $5.63 Amman, Jordan</t>
-  </si>
-  <si>
-    <t>$2.94 – $5.35 Krakow, Poland</t>
-  </si>
-  <si>
-    <t>$3.00 – $4.00 Santa Ana, El Salvador</t>
-  </si>
-  <si>
-    <t>$3.00 – $5.00 Panama City, Panama</t>
-  </si>
-  <si>
-    <t>$3.26 – $5.80 Singapore, Singapore</t>
-  </si>
-  <si>
-    <t>$3.45 – $4.51 Santiago, Chile</t>
-  </si>
-  <si>
-    <t>$3.52 – $7.03 Moscow, Russia</t>
-  </si>
-  <si>
-    <t>$3.52 – $5.28 St. Petersburg, Russia</t>
-  </si>
-  <si>
-    <t>$3.53 – $5.77 Hong Kong, China</t>
-  </si>
-  <si>
-    <t>$3.58 – $5.97 Prague, Czech Republic</t>
-  </si>
-  <si>
-    <t>$4.00 – $10.00 New York City, USA</t>
-  </si>
-  <si>
-    <t>$4.32 – $5.98 Taipei, Taiwan</t>
-  </si>
-  <si>
-    <t>$4.49 – $6.74 Lisbon, Portugal</t>
-  </si>
-  <si>
-    <t>$4.53 – $6.20 San Jose, Costa Rica</t>
-  </si>
-  <si>
-    <t>$4.54 – $4.99 Zagreb, Croatia</t>
-  </si>
-  <si>
-    <t>$4.70 – $5.83 Budapest, Hungary</t>
-  </si>
-  <si>
-    <t>$5.31 – $7.97 Beirut, Lebanon</t>
-  </si>
-  <si>
-    <t>$5.38 – $6.73 Dar es Salaam, Tanzania</t>
-  </si>
-  <si>
-    <t>$5.62 – $7.87 Athens, Greece</t>
-  </si>
-  <si>
-    <t>$5.62 – $7.87 Madrid, Spain</t>
-  </si>
-  <si>
-    <t>$5.62 – $8.99 Tallinn, Estonia</t>
-  </si>
-  <si>
-    <t>$5.67 – $8.50 Tel Aviv, Israel</t>
-  </si>
-  <si>
-    <t>$5.93 – $9.63 Vancouver, Canada</t>
-  </si>
-  <si>
-    <t>$5.93 – $8.89 Montreal, Canada</t>
-  </si>
-  <si>
-    <t>$6.02 – $9.02 Melbourne, Australia</t>
-  </si>
-  <si>
-    <t>$6.67 – $9.63 Toronto, Canada</t>
-  </si>
-  <si>
-    <t>$6.74 – $11.24 Dublin, Ireland</t>
-  </si>
-  <si>
-    <t>$6.78 – $9.69 Nairobi, Kenya</t>
-  </si>
-  <si>
-    <t>$7.08 – $11.24 Rome, Italy</t>
-  </si>
-  <si>
-    <t>$7.50 – $11.00 Washington DC, United States</t>
-  </si>
-  <si>
-    <t>$7.66 – $10.79 Auckland, New Zealand</t>
-  </si>
-  <si>
-    <t>$7.87 – $11.24 Barcelona, Spain</t>
-  </si>
-  <si>
-    <t>$8.00 – $15.00 Orlando, United States</t>
-  </si>
-  <si>
-    <t>$8.00 – $11.00 Chicago, United States</t>
-  </si>
-  <si>
-    <t>$8.20 – $13.00 Boston, United States</t>
-  </si>
-  <si>
-    <t>$8.27 – $13.68 Sydney, Australia</t>
-  </si>
-  <si>
-    <t>$8.27 – $11.48 Stockholm, Sweden</t>
-  </si>
-  <si>
-    <t>$8.33 – $11.36 Cairns, Australia</t>
-  </si>
-  <si>
-    <t>$8.87 – $10.70 Lima, Peru</t>
-  </si>
-  <si>
-    <t>$8.99 – $11.24 Brussels, Belgium</t>
-  </si>
-  <si>
-    <t>$8.99 – $13.48 Munich, Germany</t>
-  </si>
-  <si>
-    <t>$8.99 – $13.48 Vienna, Austria</t>
-  </si>
-  <si>
-    <t>$9.08 – $11.80 Tokyo, Japan</t>
-  </si>
-  <si>
-    <t>$10.11 – $13.48 Berlin, Germany</t>
-  </si>
-  <si>
-    <t>$10.39 – $15.58 London, England</t>
-  </si>
-  <si>
-    <t>$10.39 – $10.39 Amsterdam, Netherlands</t>
-  </si>
-  <si>
-    <t>$11.00 – $15.00 Honolulu, United States</t>
-  </si>
-  <si>
-    <t>$11.00 – $15.00 San Francisco, United States</t>
-  </si>
-  <si>
-    <t>$11.22 – $11.28 Copenhagen, Denmark</t>
-  </si>
-  <si>
-    <t>$11.24 – $16.85 Paris, France</t>
-  </si>
-  <si>
-    <t>$11.24 – $16.85 Helsinki, Finland</t>
-  </si>
-  <si>
-    <t>$11.24 – $15.73 Monaco, Monaco</t>
-  </si>
-  <si>
-    <t>$11.69 – $18.18 Edinburgh, Scotland</t>
-  </si>
-  <si>
-    <t>$11.78 – $15.31 Oslo, Norway</t>
-  </si>
-  <si>
-    <t>$12.00 – $16.00 Los Angeles, USA</t>
-  </si>
-  <si>
-    <t>$12.16 – $19.26 Reykjavik, Iceland</t>
-  </si>
-  <si>
-    <t>$13.48 – $16.85 Nice, France</t>
-  </si>
-  <si>
-    <t>$15.00 – $20.00 Miami Beach, United States</t>
-  </si>
-  <si>
-    <t>$18.56 – $24.74 Zurich, Switzerland</t>
-  </si>
-  <si>
     <t>source: https://www.priceoftravel.com/555/world-taxi-prices-what-a-3-kilometer-ride-costs-in-72-big-cities/</t>
   </si>
   <si>
@@ -300,6 +36,270 @@
   </si>
   <si>
     <t>*All prices converted into US dollars on June 8, 2017</t>
+  </si>
+  <si>
+    <t>$0.82 - $1.24 Delhi, India</t>
+  </si>
+  <si>
+    <t>$0.87 - $2.90 La Paz, Bolivia</t>
+  </si>
+  <si>
+    <t>$0.88 - $1.37 Mexico City, Mexico</t>
+  </si>
+  <si>
+    <t>$0.93 - $1.40 Mumbai, India</t>
+  </si>
+  <si>
+    <t>$1.03 - $2.05 Marrakech, Morocco</t>
+  </si>
+  <si>
+    <t>$1.09 - $1.63 Antigua, Guatemala</t>
+  </si>
+  <si>
+    <t>$1.21 - $1.62 Manila, Philippines</t>
+  </si>
+  <si>
+    <t>$1.41 - $2.34 Kuala Lumpur, Malaysia</t>
+  </si>
+  <si>
+    <t>$1.43 - $2.87 Zanzibar Town, Tanzania</t>
+  </si>
+  <si>
+    <t>$1.51 - $2.26 Kuta, Bali, Indonesia</t>
+  </si>
+  <si>
+    <t>$1.54 - $2.05 Fez, Morocco</t>
+  </si>
+  <si>
+    <t>$1.59 - $2.65 Ho Chi Minh City, Vietnam</t>
+  </si>
+  <si>
+    <t>$1.76 - $2.94 Bangkok, Thailand</t>
+  </si>
+  <si>
+    <t>$1.79 - $2.68 Yangon, Myanmar</t>
+  </si>
+  <si>
+    <t>$1.79 - $2.24 Arusha, Tanzania</t>
+  </si>
+  <si>
+    <t>$1.86 - $2.32 Cape Town, South Africa</t>
+  </si>
+  <si>
+    <t>$1.91 - $2.94 Beijing, China</t>
+  </si>
+  <si>
+    <t>$1.94 - $2.77 Cairo, Egypt</t>
+  </si>
+  <si>
+    <t>$1.98 - $3.09 Hanoi, Vietnam</t>
+  </si>
+  <si>
+    <t>$2.00 - $4.00 Quito, Ecuador</t>
+  </si>
+  <si>
+    <t>$2.25 - $3.27 Dubai, UAE</t>
+  </si>
+  <si>
+    <t>$2.27 - $4.25 Istanbul, Turkey</t>
+  </si>
+  <si>
+    <t>$2.28 - $2.43 Kathmandu, Nepal</t>
+  </si>
+  <si>
+    <t>$2.30 - $3.16 Sofia, Bulgaria</t>
+  </si>
+  <si>
+    <t>$2.50 - $3.38 Shanghai, China</t>
+  </si>
+  <si>
+    <t>$2.50 - $3.13 Buenos Aires, Argentina</t>
+  </si>
+  <si>
+    <t>$2.74 - $4.88 Rio de Janeiro, Brazil</t>
+  </si>
+  <si>
+    <t>$2.76 - $5.35 Seoul, South Korea</t>
+  </si>
+  <si>
+    <t>$2.81 - $3.51 Montevideo, Uruguay</t>
+  </si>
+  <si>
+    <t>$2.82 - $5.63 Amman, Jordan</t>
+  </si>
+  <si>
+    <t>$2.94 - $5.35 Krakow, Poland</t>
+  </si>
+  <si>
+    <t>$3.00 - $4.00 Santa Ana, El Salvador</t>
+  </si>
+  <si>
+    <t>$3.00 - $5.00 Panama City, Panama</t>
+  </si>
+  <si>
+    <t>$3.26 - $5.80 Singapore, Singapore</t>
+  </si>
+  <si>
+    <t>$3.45 - $4.51 Santiago, Chile</t>
+  </si>
+  <si>
+    <t>$3.52 - $7.03 Moscow, Russia</t>
+  </si>
+  <si>
+    <t>$3.52 - $5.28 St. Petersburg, Russia</t>
+  </si>
+  <si>
+    <t>$3.53 - $5.77 Hong Kong, China</t>
+  </si>
+  <si>
+    <t>$3.58 - $5.97 Prague, Czech Republic</t>
+  </si>
+  <si>
+    <t>$4.00 - $10.00 New York City, USA</t>
+  </si>
+  <si>
+    <t>$4.32 - $5.98 Taipei, Taiwan</t>
+  </si>
+  <si>
+    <t>$4.49 - $6.74 Lisbon, Portugal</t>
+  </si>
+  <si>
+    <t>$4.53 - $6.20 San Jose, Costa Rica</t>
+  </si>
+  <si>
+    <t>$4.54 - $4.99 Zagreb, Croatia</t>
+  </si>
+  <si>
+    <t>$4.70 - $5.83 Budapest, Hungary</t>
+  </si>
+  <si>
+    <t>$5.31 - $7.97 Beirut, Lebanon</t>
+  </si>
+  <si>
+    <t>$5.38 - $6.73 Dar es Salaam, Tanzania</t>
+  </si>
+  <si>
+    <t>$5.62 - $7.87 Athens, Greece</t>
+  </si>
+  <si>
+    <t>$5.62 - $7.87 Madrid, Spain</t>
+  </si>
+  <si>
+    <t>$5.62 - $8.99 Tallinn, Estonia</t>
+  </si>
+  <si>
+    <t>$5.67 - $8.50 Tel Aviv, Israel</t>
+  </si>
+  <si>
+    <t>$5.93 - $9.63 Vancouver, Canada</t>
+  </si>
+  <si>
+    <t>$5.93 - $8.89 Montreal, Canada</t>
+  </si>
+  <si>
+    <t>$6.02 - $9.02 Melbourne, Australia</t>
+  </si>
+  <si>
+    <t>$6.67 - $9.63 Toronto, Canada</t>
+  </si>
+  <si>
+    <t>$6.74 - $11.24 Dublin, Ireland</t>
+  </si>
+  <si>
+    <t>$6.78 - $9.69 Nairobi, Kenya</t>
+  </si>
+  <si>
+    <t>$7.08 - $11.24 Rome, Italy</t>
+  </si>
+  <si>
+    <t>$7.50 - $11.00 Washington DC, United States</t>
+  </si>
+  <si>
+    <t>$7.66 - $10.79 Auckland, New Zealand</t>
+  </si>
+  <si>
+    <t>$7.87 - $11.24 Barcelona, Spain</t>
+  </si>
+  <si>
+    <t>$8.00 - $15.00 Orlando, United States</t>
+  </si>
+  <si>
+    <t>$8.00 - $11.00 Chicago, United States</t>
+  </si>
+  <si>
+    <t>$8.20 - $13.00 Boston, United States</t>
+  </si>
+  <si>
+    <t>$8.27 - $13.68 Sydney, Australia</t>
+  </si>
+  <si>
+    <t>$8.27 - $11.48 Stockholm, Sweden</t>
+  </si>
+  <si>
+    <t>$8.33 - $11.36 Cairns, Australia</t>
+  </si>
+  <si>
+    <t>$8.87 - $10.70 Lima, Peru</t>
+  </si>
+  <si>
+    <t>$8.99 - $11.24 Brussels, Belgium</t>
+  </si>
+  <si>
+    <t>$8.99 - $13.48 Munich, Germany</t>
+  </si>
+  <si>
+    <t>$8.99 - $13.48 Vienna, Austria</t>
+  </si>
+  <si>
+    <t>$9.08 - $11.80 Tokyo, Japan</t>
+  </si>
+  <si>
+    <t>$10.11 - $13.48 Berlin, Germany</t>
+  </si>
+  <si>
+    <t>$10.39 - $15.58 London, England</t>
+  </si>
+  <si>
+    <t>$10.39 - $10.39 Amsterdam, Netherlands</t>
+  </si>
+  <si>
+    <t>$11.00 - $15.00 Honolulu, United States</t>
+  </si>
+  <si>
+    <t>$11.00 - $15.00 San Francisco, United States</t>
+  </si>
+  <si>
+    <t>$11.22 - $11.28 Copenhagen, Denmark</t>
+  </si>
+  <si>
+    <t>$11.24 - $16.85 Paris, France</t>
+  </si>
+  <si>
+    <t>$11.24 - $16.85 Helsinki, Finland</t>
+  </si>
+  <si>
+    <t>$11.24 - $15.73 Monaco, Monaco</t>
+  </si>
+  <si>
+    <t>$11.69 - $18.18 Edinburgh, Scotland</t>
+  </si>
+  <si>
+    <t>$11.78 - $15.31 Oslo, Norway</t>
+  </si>
+  <si>
+    <t>$12.00 - $16.00 Los Angeles, USA</t>
+  </si>
+  <si>
+    <t>$12.16 - $19.26 Reykjavik, Iceland</t>
+  </si>
+  <si>
+    <t>$13.48 - $16.85 Nice, France</t>
+  </si>
+  <si>
+    <t>$15.00 - $20.00 Miami Beach, United States</t>
+  </si>
+  <si>
+    <t>$18.56 - $24.74 Zurich, Switzerland</t>
   </si>
 </sst>
 </file>
@@ -635,7 +635,7 @@
   <dimension ref="A1:A92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -645,457 +645,457 @@
   <sheetData>
     <row r="1" spans="1:1" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>89</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>88</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>90</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>